<commit_message>
finished, needs cleaning up and merging
</commit_message>
<xml_diff>
--- a/working_notebooks/Tang/result/hist_trans.xlsx
+++ b/working_notebooks/Tang/result/hist_trans.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>7. AHE cl interp buf</t>
   </si>
@@ -61,13 +62,46 @@
   </si>
   <si>
     <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>10. AHE cl interp buf uchar bank mod</t>
+  </si>
+  <si>
+    <t>Hist calculation (ms)</t>
+  </si>
+  <si>
+    <t>Transformation (ms)</t>
+  </si>
+  <si>
+    <t>Time on original (8MP)</t>
+  </si>
+  <si>
+    <t>Time on small (61KP)</t>
+  </si>
+  <si>
+    <t>1. HE serial</t>
+  </si>
+  <si>
+    <t>2. HE numpy</t>
+  </si>
+  <si>
+    <t>3. LHE serial</t>
+  </si>
+  <si>
+    <t>4. AHE serial</t>
+  </si>
+  <si>
+    <t>5. AHE cl buf</t>
+  </si>
+  <si>
+    <t>6. AHE cl interp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +135,16 @@
       <color rgb="FF000000"/>
       <name val="Times"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Times"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,7 +163,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -173,13 +217,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -206,6 +254,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -232,6 +281,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -808,6 +858,28 @@
         <v>289.16000000000003</v>
       </c>
     </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1">
+        <v>241.74392</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3">
+        <v>163.53752</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -817,4 +889,189 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3">
+        <v>3400</v>
+      </c>
+      <c r="E2" s="1">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3">
+        <v>360</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3">
+        <v>15000</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3">
+        <v>15000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>3.9682400000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1">
+        <v>201.05500000000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.48</v>
+      </c>
+      <c r="D7" s="3">
+        <v>208.53</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.49312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>203.62</v>
+      </c>
+      <c r="C8" s="1">
+        <v>514.47</v>
+      </c>
+      <c r="D8" s="4">
+        <v>718.09</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.3719999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>191.29</v>
+      </c>
+      <c r="C9" s="1">
+        <v>302.83</v>
+      </c>
+      <c r="D9" s="1">
+        <v>494.12</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.5419999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>203.91</v>
+      </c>
+      <c r="C10" s="1">
+        <v>289.16000000000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>493.08</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.5552000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>241.74392</v>
+      </c>
+      <c r="C11" s="3">
+        <v>399.85935999999998</v>
+      </c>
+      <c r="D11" s="1">
+        <v>399.85935999999998</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.94112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>